<commit_message>
new target customer approach
</commit_message>
<xml_diff>
--- a/dealer list.xlsx
+++ b/dealer list.xlsx
@@ -87,10 +87,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -124,22 +124,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -154,7 +147,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -168,11 +169,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -193,7 +201,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -214,23 +230,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,17 +253,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -275,187 +275,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,10 +493,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -517,17 +543,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -542,36 +562,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -593,15 +593,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -611,130 +611,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1087,18 +1087,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="3" width="18.7777777777778" style="1" customWidth="1"/>
     <col min="4" max="6" width="15.3333333333333" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="9" width="15.3333333333333" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="15.3333333333333" customWidth="1"/>
     <col min="10" max="10" width="17.5555555555556" customWidth="1"/>
     <col min="11" max="11" width="17.2222222222222" customWidth="1"/>
     <col min="12" max="12" width="15.3333333333333" customWidth="1"/>
@@ -1293,16 +1293,30 @@
       <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="5"/>
+      <c r="D6" s="5">
+        <v>29053</v>
+      </c>
+      <c r="E6" s="5">
+        <v>23345</v>
+      </c>
+      <c r="F6" s="5">
+        <v>23323</v>
+      </c>
+      <c r="G6" s="5">
+        <v>20699</v>
+      </c>
+      <c r="H6" s="5">
+        <v>20116</v>
+      </c>
+      <c r="I6" s="9">
+        <v>8085</v>
+      </c>
+      <c r="J6" s="5">
+        <v>3726</v>
+      </c>
       <c r="K6" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4359</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1315,16 +1329,30 @@
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="5"/>
+      <c r="D7" s="5">
+        <v>30505</v>
+      </c>
+      <c r="E7" s="5">
+        <v>24969</v>
+      </c>
+      <c r="F7" s="5">
+        <v>24962</v>
+      </c>
+      <c r="G7" s="5">
+        <v>22548</v>
+      </c>
+      <c r="H7" s="5">
+        <v>21789</v>
+      </c>
+      <c r="I7" s="9">
+        <v>7873</v>
+      </c>
+      <c r="J7" s="5">
+        <v>4059</v>
+      </c>
       <c r="K7" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3814</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1337,16 +1365,30 @@
       <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="5"/>
+      <c r="D8" s="5">
+        <v>24749</v>
+      </c>
+      <c r="E8" s="5">
+        <v>20447</v>
+      </c>
+      <c r="F8" s="5">
+        <v>20440</v>
+      </c>
+      <c r="G8" s="5">
+        <v>18599</v>
+      </c>
+      <c r="H8" s="5">
+        <v>18302</v>
+      </c>
+      <c r="I8" s="9">
+        <v>7458</v>
+      </c>
+      <c r="J8" s="5">
+        <v>4078</v>
+      </c>
       <c r="K8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3380</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1359,16 +1401,30 @@
       <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="5"/>
+      <c r="D9" s="5">
+        <v>24081</v>
+      </c>
+      <c r="E9" s="5">
+        <v>16290</v>
+      </c>
+      <c r="F9" s="5">
+        <v>16262</v>
+      </c>
+      <c r="G9" s="5">
+        <v>14517</v>
+      </c>
+      <c r="H9" s="5">
+        <v>13453</v>
+      </c>
+      <c r="I9" s="10">
+        <v>5272</v>
+      </c>
+      <c r="J9" s="5">
+        <v>2400</v>
+      </c>
       <c r="K9" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1523,27 +1579,27 @@
       </c>
       <c r="D15" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5708</v>
       </c>
       <c r="E15" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F15" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2624</v>
       </c>
       <c r="G15" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>583</v>
       </c>
       <c r="H15" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>12031</v>
       </c>
       <c r="I15" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>8085</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1558,27 +1614,27 @@
       </c>
       <c r="D16" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5536</v>
       </c>
       <c r="E16" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F16" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2414</v>
       </c>
       <c r="G16" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>759</v>
       </c>
       <c r="H16" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>13916</v>
       </c>
       <c r="I16" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>7873</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1593,27 +1649,27 @@
       </c>
       <c r="D17" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4302</v>
       </c>
       <c r="E17" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F17" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1841</v>
       </c>
       <c r="G17" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>297</v>
       </c>
       <c r="H17" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>10844</v>
       </c>
       <c r="I17" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>7458</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1628,27 +1684,600 @@
       </c>
       <c r="D18" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7791</v>
       </c>
       <c r="E18" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F18" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1745</v>
       </c>
       <c r="G18" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1064</v>
       </c>
       <c r="H18" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8181</v>
       </c>
       <c r="I18" s="8">
         <f t="shared" si="6"/>
+        <v>5272</v>
+      </c>
+    </row>
+    <row r="21" ht="15.15" spans="1:11">
+      <c r="A21" s="2" t="s">
         <v>0</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" ht="15.15" spans="1:11">
+      <c r="A22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="1">
+        <v>11155</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="5">
+        <v>30515</v>
+      </c>
+      <c r="E22" s="5">
+        <v>10848</v>
+      </c>
+      <c r="F22" s="5">
+        <v>8312</v>
+      </c>
+      <c r="G22" s="5">
+        <v>8309</v>
+      </c>
+      <c r="H22" s="5">
+        <v>8307</v>
+      </c>
+      <c r="I22" s="9">
+        <v>8131</v>
+      </c>
+      <c r="J22" s="5">
+        <v>3567</v>
+      </c>
+      <c r="K22" s="5">
+        <f t="shared" ref="K22:K29" si="7">I22-J22</f>
+        <v>4564</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>11171</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="5">
+        <v>30328</v>
+      </c>
+      <c r="E23" s="5">
+        <v>9031</v>
+      </c>
+      <c r="F23" s="5">
+        <v>4878</v>
+      </c>
+      <c r="G23" s="5">
+        <v>4877</v>
+      </c>
+      <c r="H23" s="5">
+        <v>4870</v>
+      </c>
+      <c r="I23" s="10">
+        <v>4716</v>
+      </c>
+      <c r="J23" s="5">
+        <v>2179</v>
+      </c>
+      <c r="K23" s="5">
+        <f t="shared" si="7"/>
+        <v>2537</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="1">
+        <v>12021</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="5">
+        <v>34682</v>
+      </c>
+      <c r="E24" s="5">
+        <v>12020</v>
+      </c>
+      <c r="F24" s="5">
+        <v>10236</v>
+      </c>
+      <c r="G24" s="5">
+        <v>10236</v>
+      </c>
+      <c r="H24" s="5">
+        <v>10235</v>
+      </c>
+      <c r="I24" s="9">
+        <v>9710</v>
+      </c>
+      <c r="J24" s="5">
+        <v>5132</v>
+      </c>
+      <c r="K24" s="5">
+        <f t="shared" si="7"/>
+        <v>4578</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="1">
+        <v>15099</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="5">
+        <v>40648</v>
+      </c>
+      <c r="E25" s="5">
+        <v>12216</v>
+      </c>
+      <c r="F25" s="5">
+        <v>9605</v>
+      </c>
+      <c r="G25" s="5">
+        <v>9601</v>
+      </c>
+      <c r="H25" s="5">
+        <v>9583</v>
+      </c>
+      <c r="I25" s="9">
+        <v>9428</v>
+      </c>
+      <c r="J25" s="5">
+        <v>5329</v>
+      </c>
+      <c r="K25" s="5">
+        <f t="shared" si="7"/>
+        <v>4099</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="1">
+        <v>13011</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="9">
+        <v>8085</v>
+      </c>
+      <c r="J26" s="5">
+        <v>3726</v>
+      </c>
+      <c r="K26" s="5">
+        <f t="shared" si="7"/>
+        <v>4359</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="1">
+        <v>13144</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="9">
+        <v>7873</v>
+      </c>
+      <c r="J27" s="5">
+        <v>4059</v>
+      </c>
+      <c r="K27" s="5">
+        <f t="shared" si="7"/>
+        <v>3814</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="1">
+        <v>16030</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="9">
+        <v>7458</v>
+      </c>
+      <c r="J28" s="5">
+        <v>4078</v>
+      </c>
+      <c r="K28" s="5">
+        <f t="shared" si="7"/>
+        <v>3380</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="1">
+        <v>16188</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="5">
+        <v>24081</v>
+      </c>
+      <c r="E29" s="5">
+        <v>7907</v>
+      </c>
+      <c r="F29" s="5">
+        <v>5467</v>
+      </c>
+      <c r="G29" s="5">
+        <v>5461</v>
+      </c>
+      <c r="H29" s="5">
+        <v>5451</v>
+      </c>
+      <c r="I29" s="10">
+        <v>5272</v>
+      </c>
+      <c r="J29" s="5">
+        <v>2400</v>
+      </c>
+      <c r="K29" s="5">
+        <f t="shared" si="7"/>
+        <v>2872</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="7">
+        <v>11155</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="8">
+        <f t="shared" ref="D31:H31" si="8">D22-E22</f>
+        <v>19667</v>
+      </c>
+      <c r="E31" s="8">
+        <f t="shared" si="8"/>
+        <v>2536</v>
+      </c>
+      <c r="F31" s="8">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="G31" s="8">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="H31" s="8">
+        <f t="shared" si="8"/>
+        <v>176</v>
+      </c>
+      <c r="I31" s="8">
+        <f t="shared" ref="I31:I38" si="9">I22</f>
+        <v>8131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="7">
+        <v>11171</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="8">
+        <f t="shared" ref="D32:H32" si="10">D23-E23</f>
+        <v>21297</v>
+      </c>
+      <c r="E32" s="8">
+        <f t="shared" si="10"/>
+        <v>4153</v>
+      </c>
+      <c r="F32" s="8">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="G32" s="8">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="H32" s="8">
+        <f t="shared" si="10"/>
+        <v>154</v>
+      </c>
+      <c r="I32" s="8">
+        <f t="shared" si="9"/>
+        <v>4716</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="7">
+        <v>12021</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="8">
+        <f t="shared" ref="D33:H33" si="11">D24-E24</f>
+        <v>22662</v>
+      </c>
+      <c r="E33" s="8">
+        <f t="shared" si="11"/>
+        <v>1784</v>
+      </c>
+      <c r="F33" s="8">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="8">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="H33" s="8">
+        <f t="shared" si="11"/>
+        <v>525</v>
+      </c>
+      <c r="I33" s="8">
+        <f t="shared" si="9"/>
+        <v>9710</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="7">
+        <v>15099</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="8">
+        <f t="shared" ref="D34:H34" si="12">D25-E25</f>
+        <v>28432</v>
+      </c>
+      <c r="E34" s="8">
+        <f t="shared" si="12"/>
+        <v>2611</v>
+      </c>
+      <c r="F34" s="8">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="G34" s="8">
+        <f t="shared" si="12"/>
+        <v>18</v>
+      </c>
+      <c r="H34" s="8">
+        <f t="shared" si="12"/>
+        <v>155</v>
+      </c>
+      <c r="I34" s="8">
+        <f t="shared" si="9"/>
+        <v>9428</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="7">
+        <v>13011</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="8">
+        <f t="shared" ref="D35:H35" si="13">D26-E26</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G35" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H35" s="8">
+        <f t="shared" si="13"/>
+        <v>-8085</v>
+      </c>
+      <c r="I35" s="8">
+        <f t="shared" si="9"/>
+        <v>8085</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="7">
+        <v>13144</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="8">
+        <f t="shared" ref="D36:H36" si="14">D27-E27</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="8">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="8">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G36" s="8">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H36" s="8">
+        <f t="shared" si="14"/>
+        <v>-7873</v>
+      </c>
+      <c r="I36" s="8">
+        <f t="shared" si="9"/>
+        <v>7873</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="7">
+        <v>16030</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="8">
+        <f t="shared" ref="D37:H37" si="15">D28-E28</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="8">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="8">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="G37" s="8">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="H37" s="8">
+        <f t="shared" si="15"/>
+        <v>-7458</v>
+      </c>
+      <c r="I37" s="8">
+        <f t="shared" si="9"/>
+        <v>7458</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="7">
+        <v>16188</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="8">
+        <f t="shared" ref="D38:H38" si="16">D29-E29</f>
+        <v>16174</v>
+      </c>
+      <c r="E38" s="8">
+        <f t="shared" si="16"/>
+        <v>2440</v>
+      </c>
+      <c r="F38" s="8">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="G38" s="8">
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="H38" s="8">
+        <f t="shared" si="16"/>
+        <v>179</v>
+      </c>
+      <c r="I38" s="8">
+        <f t="shared" si="9"/>
+        <v>5272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>